<commit_message>
Patched unstable blowup of reachable set and commited prelim results on determinstic strat performance
</commit_message>
<xml_diff>
--- a/figures/SlidingPCAVDP with NUM_TRAJ:8000.xlsx
+++ b/figures/SlidingPCAVDP with NUM_TRAJ:8000.xlsx
@@ -449,6 +449,17 @@
           <t>SlidingPCA with Window Size:20</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>0.4723336674725943</v>
+      </c>
+      <c r="C2">
+        <f>AVERAGE(B2:B2)</f>
+        <v/>
+      </c>
+      <c r="D2">
+        <f>STDEV(B2:B2)</f>
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -456,6 +467,17 @@
           <t>SlidingPCA with Window Size:15</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>0.5149173457127998</v>
+      </c>
+      <c r="C3">
+        <f>AVERAGE(B3:B3)</f>
+        <v/>
+      </c>
+      <c r="D3">
+        <f>STDEV(B3:B3)</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -463,6 +485,17 @@
           <t>SlidingPCA with Window Size:10</t>
         </is>
       </c>
+      <c r="B4" t="n">
+        <v>0.7933767163891069</v>
+      </c>
+      <c r="C4">
+        <f>AVERAGE(B4:B4)</f>
+        <v/>
+      </c>
+      <c r="D4">
+        <f>STDEV(B4:B4)</f>
+        <v/>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -470,6 +503,17 @@
           <t>SlidingPCA with Window Size:5</t>
         </is>
       </c>
+      <c r="B6" t="n">
+        <v>5.263405291768424</v>
+      </c>
+      <c r="C6">
+        <f>AVERAGE(B6:B6)</f>
+        <v/>
+      </c>
+      <c r="D6">
+        <f>STDEV(B6:B6)</f>
+        <v/>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -477,6 +521,17 @@
           <t>SlidingPCA with Window Size:4</t>
         </is>
       </c>
+      <c r="B7" t="n">
+        <v>9.337773373270942</v>
+      </c>
+      <c r="C7">
+        <f>AVERAGE(B7:B7)</f>
+        <v/>
+      </c>
+      <c r="D7">
+        <f>STDEV(B7:B7)</f>
+        <v/>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -484,12 +539,34 @@
           <t>SlidingPCA with Window Size:3</t>
         </is>
       </c>
+      <c r="B8" t="n">
+        <v>25.85684824586824</v>
+      </c>
+      <c r="C8">
+        <f>AVERAGE(B8:B8)</f>
+        <v/>
+      </c>
+      <c r="D8">
+        <f>STDEV(B8:B8)</f>
+        <v/>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
           <t>SlidingPCA with Window Size:2</t>
         </is>
+      </c>
+      <c r="B9" t="n">
+        <v>212.5690296848721</v>
+      </c>
+      <c r="C9">
+        <f>AVERAGE(B9:B9)</f>
+        <v/>
+      </c>
+      <c r="D9">
+        <f>STDEV(B9:B9)</f>
+        <v/>
       </c>
     </row>
     <row r="10">

</xml_diff>